<commit_message>
Daily Trends V3 now active. Have grouped all data process and draw together Added active cases chart
</commit_message>
<xml_diff>
--- a/data/d_cases_by_hb.xlsx
+++ b/data/d_cases_by_hb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\githome\TTS-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC19DEC-80EE-47D6-9DAC-7FDF22D28134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6034D92-0D0F-4AD2-BFDA-43F64E06EE52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="2475" windowWidth="19875" windowHeight="11835" xr2:uid="{3A2DCE9A-1180-4B87-A40E-6C8795E2EB8B}"/>
+    <workbookView xWindow="-26020" yWindow="-4640" windowWidth="21600" windowHeight="11840" xr2:uid="{3A2DCE9A-1180-4B87-A40E-6C8795E2EB8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 - Cumulative cases" sheetId="1" r:id="rId1"/>
@@ -469,13 +469,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:Q280"/>
+  <dimension ref="A1:Q281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B252" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C253" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B280" sqref="B280"/>
+      <selection pane="bottomRight" activeCell="J281" sqref="J281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14500,6 +14500,56 @@
         <v>102.22759138249776</v>
       </c>
     </row>
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A281" s="4">
+        <v>44176</v>
+      </c>
+      <c r="B281" s="3">
+        <v>145.38661468486029</v>
+      </c>
+      <c r="C281" s="3">
+        <v>56.272184226473897</v>
+      </c>
+      <c r="D281" s="3">
+        <v>24.855568990998254</v>
+      </c>
+      <c r="E281" s="3">
+        <v>118.3241868558426</v>
+      </c>
+      <c r="F281" s="3">
+        <v>108.27028437255413</v>
+      </c>
+      <c r="G281" s="3">
+        <v>84.684992316885783</v>
+      </c>
+      <c r="H281" s="3">
+        <v>122.64182838596254</v>
+      </c>
+      <c r="I281" s="3">
+        <v>20.826857320484923</v>
+      </c>
+      <c r="J281" s="3">
+        <v>130.53331318930353</v>
+      </c>
+      <c r="K281" s="3">
+        <v>106.21653187597788</v>
+      </c>
+      <c r="L281" s="3">
+        <v>0</v>
+      </c>
+      <c r="M281" s="3">
+        <v>0</v>
+      </c>
+      <c r="N281" s="3">
+        <v>86.473279517091044</v>
+      </c>
+      <c r="O281" s="3">
+        <v>14.970059880239521</v>
+      </c>
+      <c r="P281" s="3">
+        <v>102.86822982446506</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
20th Dec Catchup - Pre Baseline
</commit_message>
<xml_diff>
--- a/data/d_cases_by_hb.xlsx
+++ b/data/d_cases_by_hb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\githome\TTS-1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DDEB4BA-3173-47E3-92B7-AD0A3A05E09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F55FEC1-82EE-4337-A3CE-3A8570819EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14775" windowHeight="11835" xr2:uid="{3A2DCE9A-1180-4B87-A40E-6C8795E2EB8B}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18240" windowHeight="11835" xr2:uid="{3A2DCE9A-1180-4B87-A40E-6C8795E2EB8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 - Cumulative cases" sheetId="1" r:id="rId1"/>
@@ -469,13 +469,13 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:Q284"/>
+  <dimension ref="A1:Q289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B264" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A284" sqref="A284:P284"/>
+      <selection pane="bottomRight" sqref="A1:P289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14700,6 +14700,256 @@
         <v>112.03851152233997</v>
       </c>
     </row>
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A285" s="4">
+        <v>44180</v>
+      </c>
+      <c r="B285" s="3">
+        <v>160.54797487546026</v>
+      </c>
+      <c r="C285" s="3">
+        <v>89.169768851181715</v>
+      </c>
+      <c r="D285" s="3">
+        <v>22.168480451430874</v>
+      </c>
+      <c r="E285" s="3">
+        <v>138.66952215232232</v>
+      </c>
+      <c r="F285" s="3">
+        <v>103.3785546569267</v>
+      </c>
+      <c r="G285" s="3">
+        <v>98.856069660235619</v>
+      </c>
+      <c r="H285" s="3">
+        <v>133.37615795523701</v>
+      </c>
+      <c r="I285" s="3">
+        <v>28.598072738576313</v>
+      </c>
+      <c r="J285" s="3">
+        <v>138.54056504003626</v>
+      </c>
+      <c r="K285" s="3">
+        <v>119.98942242006214</v>
+      </c>
+      <c r="L285" s="3">
+        <v>0</v>
+      </c>
+      <c r="M285" s="3">
+        <v>0</v>
+      </c>
+      <c r="N285" s="3">
+        <v>107.31310034253958</v>
+      </c>
+      <c r="O285" s="3">
+        <v>14.970059880239521</v>
+      </c>
+      <c r="P285" s="3">
+        <v>114.83901671151136</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A286" s="4">
+        <v>44181</v>
+      </c>
+      <c r="B286" s="3">
+        <v>167.58717782109596</v>
+      </c>
+      <c r="C286" s="3">
+        <v>91.766946584711278</v>
+      </c>
+      <c r="D286" s="3">
+        <v>19.481391911863497</v>
+      </c>
+      <c r="E286" s="3">
+        <v>133.5831883282024</v>
+      </c>
+      <c r="F286" s="3">
+        <v>96.856248369423426</v>
+      </c>
+      <c r="G286" s="3">
+        <v>96.124295714529623</v>
+      </c>
+      <c r="H286" s="3">
+        <v>123.74061802691189</v>
+      </c>
+      <c r="I286" s="3">
+        <v>29.530618588747281</v>
+      </c>
+      <c r="J286" s="3">
+        <v>130.23115274210605</v>
+      </c>
+      <c r="K286" s="3">
+        <v>118.88759117653539</v>
+      </c>
+      <c r="L286" s="3">
+        <v>0</v>
+      </c>
+      <c r="M286" s="3">
+        <v>0</v>
+      </c>
+      <c r="N286" s="3">
+        <v>106.59448583131721</v>
+      </c>
+      <c r="O286" s="3">
+        <v>14.970059880239521</v>
+      </c>
+      <c r="P286" s="3">
+        <v>111.03179397067706</v>
+      </c>
+    </row>
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A287" s="4">
+        <v>44182</v>
+      </c>
+      <c r="B287" s="3">
+        <v>162.71388347411738</v>
+      </c>
+      <c r="C287" s="3">
+        <v>91.766946584711278</v>
+      </c>
+      <c r="D287" s="3">
+        <v>24.183796856106408</v>
+      </c>
+      <c r="E287" s="3">
+        <v>128.49685450408245</v>
+      </c>
+      <c r="F287" s="3">
+        <v>84.789981737542391</v>
+      </c>
+      <c r="G287" s="3">
+        <v>102.95373057879461</v>
+      </c>
+      <c r="H287" s="3">
+        <v>124.24775170735006</v>
+      </c>
+      <c r="I287" s="3">
+        <v>34.193347839602112</v>
+      </c>
+      <c r="J287" s="3">
+        <v>126.15198670494033</v>
+      </c>
+      <c r="K287" s="3">
+        <v>117.23484431124528</v>
+      </c>
+      <c r="L287" s="3">
+        <v>0</v>
+      </c>
+      <c r="M287" s="3">
+        <v>0</v>
+      </c>
+      <c r="N287" s="3">
+        <v>101.08510791194577</v>
+      </c>
+      <c r="O287" s="3">
+        <v>0</v>
+      </c>
+      <c r="P287" s="3">
+        <v>109.65899730931855</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A288" s="4">
+        <v>44183</v>
+      </c>
+      <c r="B288" s="3">
+        <v>144.84513753519602</v>
+      </c>
+      <c r="C288" s="3">
+        <v>100.42420569647649</v>
+      </c>
+      <c r="D288" s="3">
+        <v>28.886201800349323</v>
+      </c>
+      <c r="E288" s="3">
+        <v>118.05648507562576</v>
+      </c>
+      <c r="F288" s="3">
+        <v>83.159405165666584</v>
+      </c>
+      <c r="G288" s="3">
+        <v>100.05122076148199</v>
+      </c>
+      <c r="H288" s="3">
+        <v>117.99310298194604</v>
+      </c>
+      <c r="I288" s="3">
+        <v>34.815045073049426</v>
+      </c>
+      <c r="J288" s="3">
+        <v>117.08717328901646</v>
+      </c>
+      <c r="K288" s="3">
+        <v>113.04788558584367</v>
+      </c>
+      <c r="L288" s="3">
+        <v>0</v>
+      </c>
+      <c r="M288" s="3">
+        <v>0</v>
+      </c>
+      <c r="N288" s="3">
+        <v>106.59448583131721</v>
+      </c>
+      <c r="O288" s="3">
+        <v>0</v>
+      </c>
+      <c r="P288" s="3">
+        <v>104.95488074973002</v>
+      </c>
+    </row>
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A289" s="4">
+        <v>44184</v>
+      </c>
+      <c r="B289" s="3">
+        <v>138.34741173922461</v>
+      </c>
+      <c r="C289" s="3">
+        <v>87.438317028828678</v>
+      </c>
+      <c r="D289" s="3">
+        <v>26.199113260781942</v>
+      </c>
+      <c r="E289" s="3">
+        <v>100.38816758131442</v>
+      </c>
+      <c r="F289" s="3">
+        <v>75.332637620662666</v>
+      </c>
+      <c r="G289" s="3">
+        <v>94.41693699846337</v>
+      </c>
+      <c r="H289" s="3">
+        <v>103.11718168909324</v>
+      </c>
+      <c r="I289" s="3">
+        <v>34.193347839602112</v>
+      </c>
+      <c r="J289" s="3">
+        <v>112.55476658105454</v>
+      </c>
+      <c r="K289" s="3">
+        <v>108.6405606117367</v>
+      </c>
+      <c r="L289" s="3">
+        <v>0</v>
+      </c>
+      <c r="M289" s="3">
+        <v>0</v>
+      </c>
+      <c r="N289" s="3">
+        <v>87.43143219872087</v>
+      </c>
+      <c r="O289" s="3">
+        <v>0</v>
+      </c>
+      <c r="P289" s="3">
+        <v>95.949334651218123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>